<commit_message>
perform cluster analysis of CERQ
</commit_message>
<xml_diff>
--- a/data/BackwardMask_Questionnaire_Results.xlsx
+++ b/data/BackwardMask_Questionnaire_Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juhoffmann\OneDrive - Uniklinik RWTH Aachen\Auswertung\FB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juhoffmann\Desktop\Git\UnconsciousBias\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="176">
   <si>
     <t>name</t>
   </si>
@@ -558,9 +558,6 @@
     <t>CERQ_Andere Beschuldigen</t>
   </si>
   <si>
-    <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                       </t>
-  </si>
-  <si>
     <t>BDI-II Sum score</t>
   </si>
 </sst>
@@ -965,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,7 +1037,7 @@
         <v>126</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>127</v>
@@ -1248,8 +1245,8 @@
       <c r="Z2" s="5">
         <v>7</v>
       </c>
-      <c r="AA2" s="5" t="s">
-        <v>175</v>
+      <c r="AA2" s="5">
+        <v>7</v>
       </c>
       <c r="AB2" t="s">
         <v>128</v>

</xml_diff>